<commit_message>
updated the test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/WatchlistTestData.xlsx
+++ b/src/test/test-data/WatchlistTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>API</t>
   </si>
@@ -28,9 +28,6 @@
     <t>METHOD</t>
   </si>
   <si>
-    <t>TC_T1</t>
-  </si>
-  <si>
     <t>TESTNAME</t>
   </si>
   <si>
@@ -43,76 +40,77 @@
     <t>HEADERS</t>
   </si>
   <si>
-    <t>PATHPARAMS</t>
-  </si>
-  <si>
     <t>QUERYSTRING</t>
   </si>
   <si>
     <t>BODY</t>
   </si>
   <si>
-    <t>DEPENDENCY</t>
-  </si>
-  <si>
     <t>VALIDATIONS</t>
   </si>
   <si>
     <t>STORE</t>
   </si>
   <si>
-    <t>Get Watchlist</t>
+    <t>Search for documents</t>
+  </si>
+  <si>
+    <t>1PSEARCH</t>
+  </si>
+  <si>
+    <t>?query=bio&amp;size=1</t>
+  </si>
+  <si>
+    <t>S1_TC_T1</t>
+  </si>
+  <si>
+    <t>/search</t>
+  </si>
+  <si>
+    <t>DEPENDENCYTESTS</t>
+  </si>
+  <si>
+    <t>hits.hits._id</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>S1_TC_T2</t>
   </si>
   <si>
     <t>1PCITATIONS</t>
   </si>
   <si>
+    <t>Get watchlists</t>
+  </si>
+  <si>
+    <t>/lists/watchlist</t>
+  </si>
+  <si>
     <t>x-1p-user=b58af128-88d7-4a62-85d0-0ff28f49a9c3</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Add Item to watchlist</t>
+    <t>Add new item to watchlist</t>
   </si>
   <si>
     <t>PUT</t>
   </si>
   <si>
-    <t>lists/watchlist/</t>
-  </si>
-  <si>
-    <t>Delete item from watchlist</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>Search for documents</t>
-  </si>
-  <si>
-    <t>1PSEARCH</t>
-  </si>
-  <si>
-    <t>search</t>
-  </si>
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>?query=bio&amp;size=1</t>
-  </si>
-  <si>
-    <t>{TC_T1__id}</t>
-  </si>
-  <si>
-    <t>lists/watchlist/{TC_T1__id}</t>
+    <t>S1_TC_T3</t>
+  </si>
+  <si>
+    <t>status=200</t>
+  </si>
+  <si>
+    <t>/lists/watchlist/(S1_TC_T1_hits.hits._id)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -182,7 +180,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -198,7 +196,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,38 +491,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="35.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="6" width="35.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -534,158 +530,115 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="B3" t="s">
+      <c r="K4"/>
+      <c r="L4" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6"/>
-      <c r="M6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search API test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/WatchlistTestData.xlsx
+++ b/src/test/test-data/WatchlistTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>API</t>
   </si>
@@ -104,6 +104,24 @@
   </si>
   <si>
     <t>/lists/watchlist/(S1_TC_T1_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>S1_TC_T4</t>
+  </si>
+  <si>
+    <t>S1_TC_T5</t>
+  </si>
+  <si>
+    <t>Delete item from watchlist</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>S1_TC_T6</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -491,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,6 +659,94 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated test cases for WatchList.
</commit_message>
<xml_diff>
--- a/src/test/test-data/WatchlistTestData.xlsx
+++ b/src/test/test-data/WatchlistTestData.xlsx
@@ -52,9 +52,6 @@
     <t>STORE</t>
   </si>
   <si>
-    <t>1PSEARCH</t>
-  </si>
-  <si>
     <t>?query=bio&amp;size=1</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>status=200||userId=(SYS_USER1)||items.itemId=wos::(S1_TC_T1_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>1PSEARCHV3</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
@@ -590,211 +590,211 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5"/>
       <c r="J5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7"/>
       <c r="J7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
         <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9"/>
       <c r="J9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>